<commit_message>
fixed carbon tax 6000 and ran carbon tax 12000
</commit_message>
<xml_diff>
--- a/carbon-tax-6000-simulation.xlsx
+++ b/carbon-tax-6000-simulation.xlsx
@@ -868,16 +868,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>8180.6709505246</v>
+        <v>8180.672358241889</v>
       </c>
       <c r="C26" t="n">
-        <v>3503.329095744391</v>
+        <v>3503.329021111389</v>
       </c>
       <c r="D26" t="n">
         <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>37.77651943586419</v>
+        <v>39.06802240957155</v>
       </c>
     </row>
     <row r="27">
@@ -885,16 +885,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>8445.694471044881</v>
+        <v>8445.696297761351</v>
       </c>
       <c r="C27" t="n">
-        <v>2768.305542926201</v>
+        <v>2768.305446081976</v>
       </c>
       <c r="D27" t="n">
-        <v>2.933188635189234e-07</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>44.21235255929208</v>
+        <v>40.56898989358593</v>
       </c>
     </row>
     <row r="28">
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>7671.608631032938</v>
+        <v>7671.607662584925</v>
       </c>
       <c r="C28" t="n">
-        <v>3328.391462304583</v>
+        <v>3328.391902945671</v>
       </c>
       <c r="D28" t="n">
-        <v>0</v>
+        <v>0.0004340354369779062</v>
       </c>
       <c r="E28" t="n">
-        <v>37.56514570942686</v>
+        <v>37.88692089365129</v>
       </c>
     </row>
     <row r="29">
@@ -919,16 +919,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>8023.257681656675</v>
+        <v>8023.261470738268</v>
       </c>
       <c r="C29" t="n">
-        <v>2917.742382744687</v>
+        <v>2917.74218187625</v>
       </c>
       <c r="D29" t="n">
         <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>40.56300731092108</v>
+        <v>39.4731408055999</v>
       </c>
     </row>
     <row r="30">
@@ -936,16 +936,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>8723.218361972764</v>
+        <v>8723.218088557071</v>
       </c>
       <c r="C30" t="n">
-        <v>2515.781578455844</v>
+        <v>2515.781713531522</v>
       </c>
       <c r="D30" t="n">
-        <v>5.951188633489641e-05</v>
+        <v>0.0001977138280283951</v>
       </c>
       <c r="E30" t="n">
-        <v>44.40889981641291</v>
+        <v>44.81633191842522</v>
       </c>
     </row>
     <row r="31">
@@ -953,16 +953,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>8888.321494693961</v>
+        <v>8888.328385634313</v>
       </c>
       <c r="C31" t="n">
-        <v>3448.678165587116</v>
+        <v>3448.677502794083</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0003393793887691104</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>39.56488197524272</v>
+        <v>41.24225219482881</v>
       </c>
     </row>
     <row r="32">
@@ -970,16 +970,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>11264.99783936697</v>
+        <v>11264.97897521768</v>
       </c>
       <c r="C32" t="n">
-        <v>3077.024387228765</v>
+        <v>3077.025708594811</v>
       </c>
       <c r="D32" t="n">
         <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>63.50308680213894</v>
+        <v>63.73337790669514</v>
       </c>
     </row>
     <row r="33">
@@ -987,16 +987,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>13574.49046033314</v>
+        <v>13574.48561451635</v>
       </c>
       <c r="C33" t="n">
-        <v>2339.639286994364</v>
+        <v>2339.639735936503</v>
       </c>
       <c r="D33" t="n">
         <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>71.59433901715583</v>
+        <v>71.56626359656426</v>
       </c>
     </row>
     <row r="34">
@@ -1004,16 +1004,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>14014.85791355533</v>
+        <v>14014.87384465257</v>
       </c>
       <c r="C34" t="n">
-        <v>2398.130214346585</v>
+        <v>2398.122273553396</v>
       </c>
       <c r="D34" t="n">
-        <v>0.01186025313810769</v>
+        <v>0.003877917366315577</v>
       </c>
       <c r="E34" t="n">
-        <v>71.57921316167813</v>
+        <v>71.68280741351471</v>
       </c>
     </row>
     <row r="35">
@@ -1021,16 +1021,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>14637.49348862792</v>
+        <v>14637.55148323597</v>
       </c>
       <c r="C35" t="n">
-        <v>1947.506230877589</v>
+        <v>1947.500408116019</v>
       </c>
       <c r="D35" t="n">
-        <v>0.0002802164660457501</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>101.793957807277</v>
+        <v>101.8041085348393</v>
       </c>
     </row>
     <row r="36">
@@ -1038,16 +1038,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>15220.18468337108</v>
+        <v>15220.1896626907</v>
       </c>
       <c r="C36" t="n">
-        <v>1471.116989523412</v>
+        <v>1471.116808197464</v>
       </c>
       <c r="D36" t="n">
         <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>275.1672929770114</v>
+        <v>404.6058251525826</v>
       </c>
     </row>
     <row r="37">
@@ -1055,16 +1055,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>15189.29558522986</v>
+        <v>15189.26185943057</v>
       </c>
       <c r="C37" t="n">
-        <v>1461.705937381635</v>
+        <v>1461.722152558365</v>
       </c>
       <c r="D37" t="n">
-        <v>0</v>
+        <v>0.01597203956848309</v>
       </c>
       <c r="E37" t="n">
-        <v>104.1572748416236</v>
+        <v>104.0774390580534</v>
       </c>
     </row>
     <row r="38">
@@ -1072,16 +1072,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>14754.80132338772</v>
+        <v>14754.87729288981</v>
       </c>
       <c r="C38" t="n">
-        <v>1724.198026168497</v>
+        <v>1724.18995100689</v>
       </c>
       <c r="D38" t="n">
-        <v>0.0006497926630256297</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>102.2110317849688</v>
+        <v>102.2897637972766</v>
       </c>
     </row>
     <row r="39">
@@ -1089,16 +1089,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>14173.54865924492</v>
+        <v>14173.54706033345</v>
       </c>
       <c r="C39" t="n">
-        <v>2193.451958352411</v>
+        <v>2193.452479291771</v>
       </c>
       <c r="D39" t="n">
-        <v>0</v>
+        <v>0.0004599149015279558</v>
       </c>
       <c r="E39" t="n">
-        <v>74.36886094130489</v>
+        <v>74.37213189178445</v>
       </c>
     </row>
     <row r="40">
@@ -1106,16 +1106,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>13667.05686137586</v>
+        <v>13667.06016139133</v>
       </c>
       <c r="C40" t="n">
-        <v>2505.94327897824</v>
+        <v>2505.943207030746</v>
       </c>
       <c r="D40" t="n">
         <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>71.43525987846861</v>
+        <v>71.43550013523983</v>
       </c>
     </row>
     <row r="41">
@@ -1123,16 +1123,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>13397.53821266293</v>
+        <v>13397.53817610087</v>
       </c>
       <c r="C41" t="n">
-        <v>2696.461795534097</v>
+        <v>2696.461811413106</v>
       </c>
       <c r="D41" t="n">
-        <v>0</v>
+        <v>1.247353378984304e-05</v>
       </c>
       <c r="E41" t="n">
-        <v>70.64981708309955</v>
+        <v>70.64968577912155</v>
       </c>
     </row>
     <row r="42">
@@ -1140,16 +1140,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>13468.80710206579</v>
+        <v>13468.8070998825</v>
       </c>
       <c r="C42" t="n">
-        <v>2756.192897301645</v>
+        <v>2756.192900367333</v>
       </c>
       <c r="D42" t="n">
-        <v>6.635745167222747e-07</v>
+        <v>8.368226540230149e-07</v>
       </c>
       <c r="E42" t="n">
-        <v>70.81978563869622</v>
+        <v>70.81983415978519</v>
       </c>
     </row>
     <row r="43">
@@ -1157,16 +1157,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>13469.04808102572</v>
+        <v>13469.04807645426</v>
       </c>
       <c r="C43" t="n">
-        <v>3043.951925969618</v>
+        <v>3043.951927405258</v>
       </c>
       <c r="D43" t="n">
-        <v>4.411749138619031e-07</v>
+        <v>4.150775471680627e-08</v>
       </c>
       <c r="E43" t="n">
-        <v>70.82034898798136</v>
+        <v>70.82032963178303</v>
       </c>
     </row>
     <row r="44">
@@ -1174,16 +1174,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>13849.7953769978</v>
+        <v>13849.79539189354</v>
       </c>
       <c r="C44" t="n">
-        <v>3152.204622709027</v>
+        <v>3152.204621137435</v>
       </c>
       <c r="D44" t="n">
-        <v>4.977689217046463e-07</v>
+        <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>71.77989122363084</v>
+        <v>71.77990148550442</v>
       </c>
     </row>
     <row r="45">
@@ -1191,16 +1191,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>13754.02548135879</v>
+        <v>13754.02553260137</v>
       </c>
       <c r="C45" t="n">
-        <v>2969.97451864258</v>
+        <v>2969.974513903791</v>
       </c>
       <c r="D45" t="n">
-        <v>4.646858652539369e-07</v>
+        <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>71.74714861741013</v>
+        <v>71.74715312639759</v>
       </c>
     </row>
     <row r="46">
@@ -1208,16 +1208,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>13653.32238299331</v>
+        <v>13653.32226281086</v>
       </c>
       <c r="C46" t="n">
-        <v>2427.677671592799</v>
+        <v>2427.67770651404</v>
       </c>
       <c r="D46" t="n">
-        <v>0</v>
+        <v>3.064448357956724e-05</v>
       </c>
       <c r="E46" t="n">
-        <v>71.6565142826141</v>
+        <v>71.65654256392229</v>
       </c>
     </row>
     <row r="47">
@@ -1225,16 +1225,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>12639.84005797085</v>
+        <v>12639.84281598591</v>
       </c>
       <c r="C47" t="n">
-        <v>2537.159908034115</v>
+        <v>2537.159684981272</v>
       </c>
       <c r="D47" t="n">
-        <v>3.396104770171522e-05</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>70.70345727264584</v>
+        <v>70.70301339812373</v>
       </c>
     </row>
     <row r="48">
@@ -1242,16 +1242,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>11560.09003819341</v>
+        <v>11560.08772187614</v>
       </c>
       <c r="C48" t="n">
-        <v>2312.909917940327</v>
+        <v>2312.911078276927</v>
       </c>
       <c r="D48" t="n">
-        <v>4.382243052312218e-05</v>
+        <v>0.001198648385969982</v>
       </c>
       <c r="E48" t="n">
-        <v>69.72202419720814</v>
+        <v>69.70223334004751</v>
       </c>
     </row>
     <row r="49">
@@ -1259,16 +1259,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>10267.32881360739</v>
+        <v>10267.32879663119</v>
       </c>
       <c r="C49" t="n">
-        <v>2332.671186296943</v>
+        <v>2332.671194806387</v>
       </c>
       <c r="D49" t="n">
-        <v>3.126476315272542e-07</v>
+        <v>8.553855339846579e-06</v>
       </c>
       <c r="E49" t="n">
-        <v>47.26855177220011</v>
+        <v>47.26843578310506</v>
       </c>
     </row>
     <row r="50">
@@ -1276,16 +1276,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>9175.243309000349</v>
+        <v>9175.168072257264</v>
       </c>
       <c r="C50" t="n">
-        <v>2513.827553810923</v>
+        <v>2513.831851109669</v>
       </c>
       <c r="D50" t="n">
-        <v>0</v>
+        <v>7.655654652166007e-05</v>
       </c>
       <c r="E50" t="n">
-        <v>40.37681096147038</v>
+        <v>41.2639914580156</v>
       </c>
     </row>
     <row r="51">
@@ -1293,16 +1293,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>8653.594202438368</v>
+        <v>8653.501405610086</v>
       </c>
       <c r="C51" t="n">
-        <v>2497.51348021009</v>
+        <v>2497.519116745622</v>
       </c>
       <c r="D51" t="n">
         <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>39.84394266031087</v>
+        <v>40.23187591319846</v>
       </c>
     </row>
     <row r="52">
@@ -1310,16 +1310,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>9297.633233820668</v>
+        <v>9297.639339773199</v>
       </c>
       <c r="C52" t="n">
-        <v>1556.361082800821</v>
+        <v>1556.357959378087</v>
       </c>
       <c r="D52" t="n">
-        <v>0.005677727336137185</v>
+        <v>0.002698151512766097</v>
       </c>
       <c r="E52" t="n">
-        <v>44.35758248038532</v>
+        <v>44.3963858844789</v>
       </c>
     </row>
     <row r="53">
@@ -1327,16 +1327,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>9519.102652495287</v>
+        <v>9518.896268458755</v>
       </c>
       <c r="C53" t="n">
-        <v>1209.089997738592</v>
+        <v>1209.102576633152</v>
       </c>
       <c r="D53" t="n">
-        <v>0</v>
+        <v>0.001153754859595183</v>
       </c>
       <c r="E53" t="n">
-        <v>44.46160575405359</v>
+        <v>44.47849963995908</v>
       </c>
     </row>
     <row r="54">
@@ -1344,16 +1344,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>9395.869154359136</v>
+        <v>9395.919214459971</v>
       </c>
       <c r="C54" t="n">
-        <v>1409.106063438831</v>
+        <v>1409.080956453652</v>
       </c>
       <c r="D54" t="n">
-        <v>0.02475744939353718</v>
+        <v>2.327711806377779e-05</v>
       </c>
       <c r="E54" t="n">
-        <v>44.39705695268742</v>
+        <v>44.41270244697179</v>
       </c>
     </row>
     <row r="55">
@@ -1361,16 +1361,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>9404.293671752936</v>
+        <v>9404.340064931748</v>
       </c>
       <c r="C55" t="n">
-        <v>1745.702156246633</v>
+        <v>1745.695836181713</v>
       </c>
       <c r="D55" t="n">
-        <v>0.004167870859725104</v>
+        <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>44.26989347227954</v>
+        <v>44.40207474602661</v>
       </c>
     </row>
     <row r="56">
@@ -1378,16 +1378,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>10284.81742827886</v>
+        <v>10284.79480486116</v>
       </c>
       <c r="C56" t="n">
-        <v>1574.203581490164</v>
+        <v>1574.204888214488</v>
       </c>
       <c r="D56" t="n">
-        <v>0</v>
+        <v>0.0003066177833012983</v>
       </c>
       <c r="E56" t="n">
-        <v>48.18293756657199</v>
+        <v>48.88707735332508</v>
       </c>
     </row>
     <row r="57">
@@ -1395,16 +1395,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>11693.1202383641</v>
+        <v>11693.11943223559</v>
       </c>
       <c r="C57" t="n">
-        <v>1375.880661957335</v>
+        <v>1375.881297444914</v>
       </c>
       <c r="D57" t="n">
         <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>69.39305911648221</v>
+        <v>69.44085935263706</v>
       </c>
     </row>
     <row r="58">
@@ -1412,16 +1412,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>12623.28740850782</v>
+        <v>12623.28809277375</v>
       </c>
       <c r="C58" t="n">
-        <v>1614.71220984134</v>
+        <v>1614.711893819308</v>
       </c>
       <c r="D58" t="n">
-        <v>0.0003812663540963676</v>
+        <v>1.402836671184994e-05</v>
       </c>
       <c r="E58" t="n">
-        <v>70.22465138283712</v>
+        <v>70.21828036001628</v>
       </c>
     </row>
     <row r="59">
@@ -1429,16 +1429,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>13571.55821694434</v>
+        <v>13571.55226520094</v>
       </c>
       <c r="C59" t="n">
-        <v>1430.448039007199</v>
+        <v>1430.448466352834</v>
       </c>
       <c r="D59" t="n">
         <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>71.24414579308454</v>
+        <v>71.25371049461847</v>
       </c>
     </row>
     <row r="60">
@@ -1446,16 +1446,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>13852.71189022789</v>
+        <v>13852.71217655537</v>
       </c>
       <c r="C60" t="n">
-        <v>1383.287973376529</v>
+        <v>1383.287801749875</v>
       </c>
       <c r="D60" t="n">
-        <v>0.0001362640598416918</v>
+        <v>2.16731324247075e-05</v>
       </c>
       <c r="E60" t="n">
-        <v>71.6535445262323</v>
+        <v>71.6513129385396</v>
       </c>
     </row>
     <row r="61">
@@ -1463,16 +1463,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>13902.4562815414</v>
+        <v>13902.45635035105</v>
       </c>
       <c r="C61" t="n">
-        <v>1310.543678146812</v>
+        <v>1310.54363302941</v>
       </c>
       <c r="D61" t="n">
-        <v>4.027255559948814e-05</v>
+        <v>1.660295766228456e-05</v>
       </c>
       <c r="E61" t="n">
-        <v>71.82499408121274</v>
+        <v>71.82489806192326</v>
       </c>
     </row>
     <row r="62">
@@ -1480,16 +1480,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>13886.03716083144</v>
+        <v>13886.03669161701</v>
       </c>
       <c r="C62" t="n">
-        <v>1063.963430152205</v>
+        <v>1063.963464010142</v>
       </c>
       <c r="D62" t="n">
         <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>71.78411072408026</v>
+        <v>71.78356415182147</v>
       </c>
     </row>
     <row r="63">
@@ -1497,16 +1497,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>13897.98390352133</v>
+        <v>13897.98411646945</v>
       </c>
       <c r="C63" t="n">
-        <v>728.0164596942375</v>
+        <v>728.0164484110375</v>
       </c>
       <c r="D63" t="n">
         <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>71.83104442088577</v>
+        <v>71.83435659416584</v>
       </c>
     </row>
     <row r="64">
@@ -1514,16 +1514,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>13767.97691850338</v>
+        <v>13767.97699214777</v>
       </c>
       <c r="C64" t="n">
-        <v>583.0230490390782</v>
+        <v>583.0230142605637</v>
       </c>
       <c r="D64" t="n">
-        <v>3.242544957079005e-05</v>
+        <v>3.912190843848215e-07</v>
       </c>
       <c r="E64" t="n">
-        <v>71.70213019919797</v>
+        <v>71.69948791067819</v>
       </c>
     </row>
     <row r="65">
@@ -1531,16 +1531,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>13730.60792170761</v>
+        <v>13730.60934967132</v>
       </c>
       <c r="C65" t="n">
-        <v>503.3920178049123</v>
+        <v>503.3918521423201</v>
       </c>
       <c r="D65" t="n">
-        <v>6.042730930789207e-05</v>
+        <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>71.72644835016227</v>
+        <v>71.72805278210538</v>
       </c>
     </row>
     <row r="66">
@@ -1548,16 +1548,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>13828.40582666088</v>
+        <v>13828.40539125703</v>
       </c>
       <c r="C66" t="n">
-        <v>653.5941417164859</v>
+        <v>653.5943671710436</v>
       </c>
       <c r="D66" t="n">
-        <v>3.15908656784932e-05</v>
+        <v>0.0002413308254127334</v>
       </c>
       <c r="E66" t="n">
-        <v>71.76759135231053</v>
+        <v>71.76539204814486</v>
       </c>
     </row>
     <row r="67">
@@ -1565,16 +1565,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>13789.26336004453</v>
+        <v>13789.25339038018</v>
       </c>
       <c r="C67" t="n">
-        <v>1194.744142107402</v>
+        <v>1194.745760680069</v>
       </c>
       <c r="D67" t="n">
-        <v>0</v>
+        <v>0.0008480918513148936</v>
       </c>
       <c r="E67" t="n">
-        <v>71.61916481848348</v>
+        <v>71.64154097979529</v>
       </c>
     </row>
     <row r="68">
@@ -1582,16 +1582,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>13019.9578175687</v>
+        <v>13019.97499106981</v>
       </c>
       <c r="C68" t="n">
-        <v>2611.042119942586</v>
+        <v>2611.040663746931</v>
       </c>
       <c r="D68" t="n">
-        <v>6.242672821766041e-05</v>
+        <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>70.28829604507884</v>
+        <v>70.29031342079359</v>
       </c>
     </row>
     <row r="69">
@@ -1599,16 +1599,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>11909.82215155078</v>
+        <v>11909.81434939735</v>
       </c>
       <c r="C69" t="n">
-        <v>3584.184351795147</v>
+        <v>3584.185400026069</v>
       </c>
       <c r="D69" t="n">
-        <v>0</v>
+        <v>0.0004094331600554484</v>
       </c>
       <c r="E69" t="n">
-        <v>69.22802102455215</v>
+        <v>69.23448574932753</v>
       </c>
     </row>
     <row r="70">
@@ -1616,16 +1616,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>10886.2674222814</v>
+        <v>10886.31716019452</v>
       </c>
       <c r="C70" t="n">
-        <v>4082.707585893633</v>
+        <v>4082.682687293775</v>
       </c>
       <c r="D70" t="n">
-        <v>0.02496687025024805</v>
+        <v>0.0001523595702662382</v>
       </c>
       <c r="E70" t="n">
-        <v>62.10939564590272</v>
+        <v>62.33810409490127</v>
       </c>
     </row>
     <row r="71">
@@ -1633,16 +1633,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>9792.526694121496</v>
+        <v>9792.53852324863</v>
       </c>
       <c r="C71" t="n">
-        <v>4405.491975393894</v>
+        <v>4405.49110094276</v>
       </c>
       <c r="D71" t="n">
         <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>46.09655413968915</v>
+        <v>45.48246607777929</v>
       </c>
     </row>
     <row r="72">
@@ -1650,16 +1650,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>8643.363433487535</v>
+        <v>8643.341640678127</v>
       </c>
       <c r="C72" t="n">
-        <v>4535.6431525552</v>
+        <v>4535.650233057275</v>
       </c>
       <c r="D72" t="n">
-        <v>0.001087256733836386</v>
+        <v>0.008118147429487511</v>
       </c>
       <c r="E72" t="n">
-        <v>44.1862451158158</v>
+        <v>44.13358577198608</v>
       </c>
     </row>
     <row r="73">
@@ -1667,16 +1667,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>8589.501469200899</v>
+        <v>8589.833694762576</v>
       </c>
       <c r="C73" t="n">
-        <v>3529.497922085036</v>
+        <v>3529.479932930863</v>
       </c>
       <c r="D73" t="n">
-        <v>0.0006081067197704483</v>
+        <v>0</v>
       </c>
       <c r="E73" t="n">
-        <v>44.46791212014164</v>
+        <v>44.48973682062135</v>
       </c>
     </row>
     <row r="74">
@@ -1684,16 +1684,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>8648.68116533576</v>
+        <v>8648.694230910347</v>
       </c>
       <c r="C74" t="n">
-        <v>2548.329235073037</v>
+        <v>2548.326705481686</v>
       </c>
       <c r="D74" t="n">
         <v>0</v>
       </c>
       <c r="E74" t="n">
-        <v>44.22166939501908</v>
+        <v>44.88331126905538</v>
       </c>
     </row>
     <row r="75">
@@ -1701,16 +1701,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>8143.370144418674</v>
+        <v>8143.373089491341</v>
       </c>
       <c r="C75" t="n">
-        <v>2125.64221644076</v>
+        <v>2125.639557926042</v>
       </c>
       <c r="D75" t="n">
-        <v>0.002469274894256581</v>
+        <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>40.75697295838863</v>
+        <v>40.17372876518235</v>
       </c>
     </row>
     <row r="76">
@@ -1718,16 +1718,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>8952.191529506152</v>
+        <v>8951.57331169594</v>
       </c>
       <c r="C76" t="n">
-        <v>1659.389496888559</v>
+        <v>1659.425332099264</v>
       </c>
       <c r="D76" t="n">
-        <v>0</v>
+        <v>0.00135484993839039</v>
       </c>
       <c r="E76" t="n">
-        <v>44.38210131173918</v>
+        <v>48.28844359447704</v>
       </c>
     </row>
     <row r="77">
@@ -1735,16 +1735,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>9075.879327190642</v>
+        <v>9076.951715923453</v>
       </c>
       <c r="C77" t="n">
-        <v>1250.160335064158</v>
+        <v>1250.056510129812</v>
       </c>
       <c r="D77" t="n">
-        <v>0.0001441648121964461</v>
+        <v>0</v>
       </c>
       <c r="E77" t="n">
-        <v>44.28216543563331</v>
+        <v>2215.862723846444</v>
       </c>
     </row>
     <row r="78">
@@ -1752,16 +1752,16 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>8888.83280655073</v>
+        <v>8888.82353141547</v>
       </c>
       <c r="C78" t="n">
-        <v>1373.175752577704</v>
+        <v>1373.175734962159</v>
       </c>
       <c r="D78" t="n">
-        <v>0.0006805354528419644</v>
+        <v>0.0007328895110130468</v>
       </c>
       <c r="E78" t="n">
-        <v>42.16135003257026</v>
+        <v>44.43317901711924</v>
       </c>
     </row>
     <row r="79">
@@ -1769,16 +1769,16 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>8811.565503750895</v>
+        <v>8811.583886819508</v>
       </c>
       <c r="C79" t="n">
-        <v>1569.433955526926</v>
+        <v>1569.432191719062</v>
       </c>
       <c r="D79" t="n">
-        <v>0.0005402440538112762</v>
+        <v>0</v>
       </c>
       <c r="E79" t="n">
-        <v>41.35004467603527</v>
+        <v>44.32349045630093</v>
       </c>
     </row>
     <row r="80">
@@ -1786,16 +1786,16 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>9023.701251613013</v>
+        <v>9023.665089462495</v>
       </c>
       <c r="C80" t="n">
-        <v>1653.332079760909</v>
+        <v>1653.334883364324</v>
       </c>
       <c r="D80" t="n">
-        <v>0</v>
+        <v>9.547018907052946e-05</v>
       </c>
       <c r="E80" t="n">
-        <v>42.59974378618393</v>
+        <v>44.54789504041335</v>
       </c>
     </row>
     <row r="81">
@@ -1803,16 +1803,16 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>9633.525237685799</v>
+        <v>9633.570240835725</v>
       </c>
       <c r="C81" t="n">
-        <v>1540.451770072468</v>
+        <v>1540.429541624039</v>
       </c>
       <c r="D81" t="n">
-        <v>0.02296931671875885</v>
+        <v>0.0002173229344243239</v>
       </c>
       <c r="E81" t="n">
-        <v>44.46614918116389</v>
+        <v>46.80714399141673</v>
       </c>
     </row>
     <row r="82">
@@ -1820,16 +1820,16 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>10462.90027217068</v>
+        <v>10462.78759977064</v>
       </c>
       <c r="C82" t="n">
-        <v>1596.205403824803</v>
+        <v>1596.212803007534</v>
       </c>
       <c r="D82" t="n">
-        <v>0</v>
+        <v>0.0001005428560503427</v>
       </c>
       <c r="E82" t="n">
-        <v>49.4318619987525</v>
+        <v>48.76569189430331</v>
       </c>
     </row>
     <row r="83">
@@ -1837,16 +1837,16 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>11954.34073866086</v>
+        <v>11954.23764410963</v>
       </c>
       <c r="C83" t="n">
-        <v>1000.800815350827</v>
+        <v>1000.811001837116</v>
       </c>
       <c r="D83" t="n">
         <v>0</v>
       </c>
       <c r="E83" t="n">
-        <v>69.4430851177012</v>
+        <v>69.39995194939684</v>
       </c>
     </row>
     <row r="84">
@@ -1854,16 +1854,16 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>12681.11511479817</v>
+        <v>12681.1664545878</v>
       </c>
       <c r="C84" t="n">
-        <v>912.863922558608</v>
+        <v>912.8415659980251</v>
       </c>
       <c r="D84" t="n">
-        <v>0.02094174541604286</v>
+        <v>0</v>
       </c>
       <c r="E84" t="n">
-        <v>70.40854299371244</v>
+        <v>70.4222815869058</v>
       </c>
     </row>
     <row r="85">
@@ -1871,16 +1871,16 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>13031.70854949863</v>
+        <v>13031.55698403805</v>
       </c>
       <c r="C85" t="n">
-        <v>930.4264626678531</v>
+        <v>930.440121291335</v>
       </c>
       <c r="D85" t="n">
-        <v>0</v>
+        <v>0.002891779041297469</v>
       </c>
       <c r="E85" t="n">
-        <v>70.69906797674984</v>
+        <v>70.52153245128935</v>
       </c>
     </row>
     <row r="86">
@@ -1888,16 +1888,16 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>13057.84107178788</v>
+        <v>13058.18410692835</v>
       </c>
       <c r="C86" t="n">
-        <v>1043.15523798296</v>
+        <v>1043.110386435307</v>
       </c>
       <c r="D86" t="n">
-        <v>0.003686539174764437</v>
+        <v>0</v>
       </c>
       <c r="E86" t="n">
-        <v>70.76095811965573</v>
+        <v>879.3856589888024</v>
       </c>
     </row>
     <row r="87">
@@ -1905,16 +1905,16 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>12798.92839705503</v>
+        <v>12798.92922383857</v>
       </c>
       <c r="C87" t="n">
-        <v>1245.086044159653</v>
+        <v>1245.086011252423</v>
       </c>
       <c r="D87" t="n">
         <v>0</v>
       </c>
       <c r="E87" t="n">
-        <v>70.15081858885928</v>
+        <v>70.02555260353591</v>
       </c>
     </row>
     <row r="88">
@@ -1922,16 +1922,16 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>12556.61865148302</v>
+        <v>12556.61759995686</v>
       </c>
       <c r="C88" t="n">
-        <v>1340.381082267115</v>
+        <v>1340.381613602817</v>
       </c>
       <c r="D88" t="n">
-        <v>0.0002659866494645283</v>
+        <v>0.0007856548702853656</v>
       </c>
       <c r="E88" t="n">
-        <v>69.73508342858493</v>
+        <v>69.59183656840882</v>
       </c>
     </row>
     <row r="89">
@@ -1939,16 +1939,16 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>12911.72756476042</v>
+        <v>12911.72775766277</v>
       </c>
       <c r="C89" t="n">
-        <v>906.2744254571508</v>
+        <v>906.2744399895308</v>
       </c>
       <c r="D89" t="n">
         <v>0</v>
       </c>
       <c r="E89" t="n">
-        <v>70.41354941303075</v>
+        <v>70.00166124920162</v>
       </c>
     </row>
     <row r="90">
@@ -1956,16 +1956,16 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>13272.7642914286</v>
+        <v>13272.77443223526</v>
       </c>
       <c r="C90" t="n">
-        <v>771.2351755078386</v>
+        <v>771.2338483151207</v>
       </c>
       <c r="D90" t="n">
-        <v>0.0005325329722673199</v>
+        <v>0</v>
       </c>
       <c r="E90" t="n">
-        <v>70.83386193589226</v>
+        <v>70.5489328372477</v>
       </c>
     </row>
     <row r="91">
@@ -1973,16 +1973,16 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>12940.66549644548</v>
+        <v>12940.66875034574</v>
       </c>
       <c r="C91" t="n">
-        <v>1594.33389227457</v>
+        <v>1594.333127373243</v>
       </c>
       <c r="D91" t="n">
-        <v>0.0006106718724242968</v>
+        <v>0</v>
       </c>
       <c r="E91" t="n">
-        <v>70.48188200803472</v>
+        <v>70.0742934102957</v>
       </c>
     </row>
     <row r="92">
@@ -1990,16 +1990,16 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>12877.11022741503</v>
+        <v>12877.0947678736</v>
       </c>
       <c r="C92" t="n">
-        <v>2119.903029248779</v>
+        <v>2119.904474356151</v>
       </c>
       <c r="D92" t="n">
-        <v>0</v>
+        <v>0.0007570135231007927</v>
       </c>
       <c r="E92" t="n">
-        <v>70.33088543557916</v>
+        <v>69.97435807208684</v>
       </c>
     </row>
     <row r="93">
@@ -2007,16 +2007,16 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>13176.02923093987</v>
+        <v>13176.41948011921</v>
       </c>
       <c r="C93" t="n">
-        <v>2457.976847431103</v>
+        <v>2457.924159027888</v>
       </c>
       <c r="D93" t="n">
         <v>0</v>
       </c>
       <c r="E93" t="n">
-        <v>70.58895800490448</v>
+        <v>1285.075655591218</v>
       </c>
     </row>
     <row r="94">
@@ -2024,16 +2024,16 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>13053.63413584141</v>
+        <v>13053.63901120276</v>
       </c>
       <c r="C94" t="n">
-        <v>2504.365054343859</v>
+        <v>2504.363996093492</v>
       </c>
       <c r="D94" t="n">
-        <v>0.0008090069064920037</v>
+        <v>0</v>
       </c>
       <c r="E94" t="n">
-        <v>70.43956111675963</v>
+        <v>70.24670025799476</v>
       </c>
     </row>
     <row r="95">
@@ -2041,16 +2041,16 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>12556.62313988243</v>
+        <v>12557.0421499553</v>
       </c>
       <c r="C95" t="n">
-        <v>2093.37665648914</v>
+        <v>2093.326495697579</v>
       </c>
       <c r="D95" t="n">
-        <v>0.0002034003551803325</v>
+        <v>0</v>
       </c>
       <c r="E95" t="n">
-        <v>70.09021621328043</v>
+        <v>1030.400419118089</v>
       </c>
     </row>
     <row r="96">
@@ -2058,16 +2058,16 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>11495.03585627844</v>
+        <v>11495.03678200176</v>
       </c>
       <c r="C96" t="n">
-        <v>1974.964000455537</v>
+        <v>1974.963505713554</v>
       </c>
       <c r="D96" t="n">
-        <v>0.0003030947756286835</v>
+        <v>0</v>
       </c>
       <c r="E96" t="n">
-        <v>69.03614855189988</v>
+        <v>69.20573482985694</v>
       </c>
     </row>
     <row r="97">
@@ -2075,16 +2075,16 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>10104.22837541125</v>
+        <v>10104.22838736848</v>
       </c>
       <c r="C97" t="n">
-        <v>2173.771713251159</v>
+        <v>2173.771709353025</v>
       </c>
       <c r="D97" t="n">
-        <v>1.775447974307651e-06</v>
+        <v>0</v>
       </c>
       <c r="E97" t="n">
-        <v>47.14073468899028</v>
+        <v>46.96470662897995</v>
       </c>
     </row>
     <row r="98">
@@ -2092,16 +2092,16 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>9674.54742663153</v>
+        <v>9674.549489344194</v>
       </c>
       <c r="C98" t="n">
-        <v>2009.452528116349</v>
+        <v>2009.452368374651</v>
       </c>
       <c r="D98" t="n">
-        <v>4.520691272348125e-05</v>
+        <v>0</v>
       </c>
       <c r="E98" t="n">
-        <v>39.82235897107218</v>
+        <v>40.95277487121942</v>
       </c>
     </row>
     <row r="99">
@@ -2109,16 +2109,16 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>9193.662457677194</v>
+        <v>9193.662160546766</v>
       </c>
       <c r="C99" t="n">
-        <v>2020.337576086859</v>
+        <v>2020.337702632056</v>
       </c>
       <c r="D99" t="n">
-        <v>2.712708444665011e-06</v>
+        <v>0.0001366843279239024</v>
       </c>
       <c r="E99" t="n">
-        <v>39.51362983336452</v>
+        <v>39.65228715916839</v>
       </c>
     </row>
     <row r="100">
@@ -2126,16 +2126,16 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>9430.175674801218</v>
+        <v>9430.175558615549</v>
       </c>
       <c r="C100" t="n">
-        <v>1569.824297451616</v>
+        <v>1569.8243778058</v>
       </c>
       <c r="D100" t="n">
-        <v>2.771945925485655e-05</v>
+        <v>6.351572512342369e-05</v>
       </c>
       <c r="E100" t="n">
-        <v>40.97162359607547</v>
+        <v>41.23800601757065</v>
       </c>
     </row>
     <row r="101">
@@ -2143,16 +2143,16 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>9940.134041463602</v>
+        <v>9940.142548764341</v>
       </c>
       <c r="C101" t="n">
-        <v>1000.867045994053</v>
+        <v>1000.86653362103</v>
       </c>
       <c r="D101" t="n">
         <v>0</v>
       </c>
       <c r="E101" t="n">
-        <v>44.3165639830081</v>
+        <v>44.32989303180938</v>
       </c>
     </row>
     <row r="102">
@@ -2160,16 +2160,16 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>10132.75594005087</v>
+        <v>10132.75404677439</v>
       </c>
       <c r="C102" t="n">
-        <v>1106.244104959711</v>
+        <v>1106.245138699751</v>
       </c>
       <c r="D102" t="n">
-        <v>0.0001006611013245829</v>
+        <v>0.001157407822206705</v>
       </c>
       <c r="E102" t="n">
-        <v>44.33037959425121</v>
+        <v>44.32092642292189</v>
       </c>
     </row>
     <row r="103">
@@ -2177,16 +2177,16 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>11032.69855733559</v>
+        <v>11032.6954568138</v>
       </c>
       <c r="C103" t="n">
-        <v>1304.308102989975</v>
+        <v>1304.309227572699</v>
       </c>
       <c r="D103" t="n">
-        <v>0</v>
+        <v>0.0007725607768050166</v>
       </c>
       <c r="E103" t="n">
-        <v>48.50557455787858</v>
+        <v>49.34445560615751</v>
       </c>
     </row>
     <row r="104">
@@ -2194,16 +2194,16 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>12969.60683778164</v>
+        <v>12969.93783788464</v>
       </c>
       <c r="C104" t="n">
-        <v>1372.425025172322</v>
+        <v>1372.398478618575</v>
       </c>
       <c r="D104" t="n">
-        <v>0.001340177758883177</v>
+        <v>0</v>
       </c>
       <c r="E104" t="n">
-        <v>69.77383186631894</v>
+        <v>69.77085251200488</v>
       </c>
     </row>
     <row r="105">
@@ -2211,16 +2211,16 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>14607.75287224526</v>
+        <v>14607.78744108553</v>
       </c>
       <c r="C105" t="n">
-        <v>1306.926620808273</v>
+        <v>1306.92506986233</v>
       </c>
       <c r="D105" t="n">
         <v>0</v>
       </c>
       <c r="E105" t="n">
-        <v>464.9771659999298</v>
+        <v>539.7940569435812</v>
       </c>
     </row>
     <row r="106">
@@ -2228,16 +2228,16 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>15438.57428865955</v>
+        <v>15438.57271292656</v>
       </c>
       <c r="C106" t="n">
-        <v>974.4257484916837</v>
+        <v>974.4265231385165</v>
       </c>
       <c r="D106" t="n">
-        <v>0</v>
+        <v>0.0007631716893005168</v>
       </c>
       <c r="E106" t="n">
-        <v>102.2086199333474</v>
+        <v>102.1970026480619</v>
       </c>
     </row>
     <row r="107">
@@ -2245,16 +2245,16 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>15791.64258402586</v>
+        <v>15791.64305805394</v>
       </c>
       <c r="C107" t="n">
-        <v>793.7959093639288</v>
+        <v>793.7958612611112</v>
       </c>
       <c r="D107" t="n">
         <v>0</v>
       </c>
       <c r="E107" t="n">
-        <v>406.9009575923345</v>
+        <v>458.817128149218</v>
       </c>
     </row>
     <row r="108">
@@ -2262,16 +2262,16 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>15963.81395577708</v>
+        <v>15963.81398940051</v>
       </c>
       <c r="C108" t="n">
-        <v>727.1858793517672</v>
+        <v>727.185876626286</v>
       </c>
       <c r="D108" t="n">
-        <v>0.0001647064630379655</v>
+        <v>0.0001338397276022382</v>
       </c>
       <c r="E108" t="n">
-        <v>106.5498936122115</v>
+        <v>106.5392706485012</v>
       </c>
     </row>
     <row r="109">
@@ -2279,16 +2279,16 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>15962.53282214157</v>
+        <v>15962.53298762451</v>
       </c>
       <c r="C109" t="n">
-        <v>688.4683891844965</v>
+        <v>688.4684095384035</v>
       </c>
       <c r="D109" t="n">
         <v>0</v>
       </c>
       <c r="E109" t="n">
-        <v>106.517520584606</v>
+        <v>106.527412248947</v>
       </c>
     </row>
     <row r="110">
@@ -2296,16 +2296,16 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>15822.80788625766</v>
+        <v>15822.80837043547</v>
       </c>
       <c r="C110" t="n">
-        <v>656.1914618055196</v>
+        <v>656.1912162869135</v>
       </c>
       <c r="D110" t="n">
-        <v>0.0006512855542980886</v>
+        <v>0.0004128647373263766</v>
       </c>
       <c r="E110" t="n">
-        <v>103.9232762246726</v>
+        <v>103.8755205935262</v>
       </c>
     </row>
     <row r="111">
@@ -2313,16 +2313,16 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>15741.61482257191</v>
+        <v>15741.61776840377</v>
       </c>
       <c r="C111" t="n">
-        <v>625.823923752002</v>
+        <v>625.8237606712296</v>
       </c>
       <c r="D111" t="n">
         <v>0</v>
       </c>
       <c r="E111" t="n">
-        <v>407.1363131742485</v>
+        <v>492.7231995158882</v>
       </c>
     </row>
     <row r="112">
@@ -2330,16 +2330,16 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>15491.97017208472</v>
+        <v>15491.9697258559</v>
       </c>
       <c r="C112" t="n">
-        <v>681.0297104611627</v>
+        <v>681.0299321999172</v>
       </c>
       <c r="D112" t="n">
-        <v>0.0001173367719774067</v>
+        <v>0.0003416025765015377</v>
       </c>
       <c r="E112" t="n">
-        <v>102.3182380913333</v>
+        <v>102.297076311728</v>
       </c>
     </row>
     <row r="113">
@@ -2347,16 +2347,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>15432.22599314856</v>
+        <v>15432.22651077527</v>
       </c>
       <c r="C113" t="n">
-        <v>661.7737315522841</v>
+        <v>661.7734743852511</v>
       </c>
       <c r="D113" t="n">
-        <v>0.0002750241258794995</v>
+        <v>1.482470449992482e-05</v>
       </c>
       <c r="E113" t="n">
-        <v>102.1213457974402</v>
+        <v>102.1110426481539</v>
       </c>
     </row>
     <row r="114">
@@ -2364,16 +2364,16 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>15327.98385604774</v>
+        <v>15327.98492790531</v>
       </c>
       <c r="C114" t="n">
-        <v>897.0157802751451</v>
+        <v>897.0153780887243</v>
       </c>
       <c r="D114" t="n">
-        <v>0.0003633138344242451</v>
+        <v>0</v>
       </c>
       <c r="E114" t="n">
-        <v>101.7690281887989</v>
+        <v>101.7570511042926</v>
       </c>
     </row>
     <row r="115">
@@ -2381,16 +2381,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>15010.02192392296</v>
+        <v>15010.02199153373</v>
       </c>
       <c r="C115" t="n">
-        <v>1502.978130970675</v>
+        <v>1502.978126419661</v>
       </c>
       <c r="D115" t="n">
         <v>0</v>
       </c>
       <c r="E115" t="n">
-        <v>73.87585666316097</v>
+        <v>73.83649423211553</v>
       </c>
     </row>
     <row r="116">
@@ -2398,16 +2398,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>15680.0608038296</v>
+        <v>15680.06018864706</v>
       </c>
       <c r="C116" t="n">
-        <v>1321.93957542436</v>
+        <v>1321.939715674978</v>
       </c>
       <c r="D116" t="n">
-        <v>0</v>
+        <v>9.558241212445875e-05</v>
       </c>
       <c r="E116" t="n">
-        <v>103.1536635303707</v>
+        <v>103.1524521082985</v>
       </c>
     </row>
     <row r="117">
@@ -2415,16 +2415,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>15867.83845463789</v>
+        <v>15867.83862526479</v>
       </c>
       <c r="C117" t="n">
-        <v>856.6863806685607</v>
+        <v>856.6863725959757</v>
       </c>
       <c r="D117" t="n">
         <v>0</v>
       </c>
       <c r="E117" t="n">
-        <v>261.7562384985243</v>
+        <v>339.7536794132629</v>
       </c>
     </row>
     <row r="118">
@@ -2432,16 +2432,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>15614.13021373959</v>
+        <v>15614.12960825746</v>
       </c>
       <c r="C118" t="n">
-        <v>467.5728931092779</v>
+        <v>467.5729284391148</v>
       </c>
       <c r="D118" t="n">
         <v>0</v>
       </c>
       <c r="E118" t="n">
-        <v>209.6872306982664</v>
+        <v>288.2603926332109</v>
       </c>
     </row>
     <row r="119">
@@ -2449,16 +2449,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>14786.95649793331</v>
+        <v>14786.95723646862</v>
       </c>
       <c r="C119" t="n">
-        <v>390.0873334545041</v>
+        <v>390.0872431936858</v>
       </c>
       <c r="D119" t="n">
-        <v>2.701988753463752e-05</v>
+        <v>0</v>
       </c>
       <c r="E119" t="n">
-        <v>81.26383154473061</v>
+        <v>81.2635594564786</v>
       </c>
     </row>
     <row r="120">
@@ -2466,16 +2466,16 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>13596.78760135311</v>
+        <v>13596.78758162564</v>
       </c>
       <c r="C120" t="n">
-        <v>276.2123962843807</v>
+        <v>276.2124071549541</v>
       </c>
       <c r="D120" t="n">
-        <v>2.360136503306736e-06</v>
+        <v>1.314316466800181e-05</v>
       </c>
       <c r="E120" t="n">
-        <v>71.1123181493279</v>
+        <v>71.72496660434705</v>
       </c>
     </row>
     <row r="121">
@@ -2483,16 +2483,16 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>12322.61586650152</v>
+        <v>12322.6159956478</v>
       </c>
       <c r="C121" t="n">
-        <v>277.3841339896079</v>
+        <v>277.384125458155</v>
       </c>
       <c r="D121" t="n">
-        <v>1.335957462922013e-07</v>
+        <v>0</v>
       </c>
       <c r="E121" t="n">
-        <v>69.08226686416864</v>
+        <v>69.81981639777963</v>
       </c>
     </row>
     <row r="122">
@@ -2500,16 +2500,16 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>11416.51794840011</v>
+        <v>11416.61169142575</v>
       </c>
       <c r="C122" t="n">
-        <v>272.435223345069</v>
+        <v>272.3882773437247</v>
       </c>
       <c r="D122" t="n">
-        <v>0.04678147716667457</v>
+        <v>3.11993798523063e-05</v>
       </c>
       <c r="E122" t="n">
-        <v>63.72057959698668</v>
+        <v>63.4455864698683</v>
       </c>
     </row>
     <row r="123">
@@ -2517,16 +2517,16 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>10832.7738143611</v>
+        <v>10832.77615651353</v>
       </c>
       <c r="C123" t="n">
-        <v>318.2250163445333</v>
+        <v>318.223842742063</v>
       </c>
       <c r="D123" t="n">
-        <v>0.001168126391889567</v>
+        <v>7.436551360334231e-07</v>
       </c>
       <c r="E123" t="n">
-        <v>44.49844229129333</v>
+        <v>44.4952056213161</v>
       </c>
     </row>
     <row r="124">
@@ -2534,16 +2534,16 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>10765.71395771091</v>
+        <v>10765.71260383437</v>
       </c>
       <c r="C124" t="n">
-        <v>88.28731086250929</v>
+        <v>88.28739608293998</v>
       </c>
       <c r="D124" t="n">
-        <v>0</v>
+        <v>8.259512725282817e-08</v>
       </c>
       <c r="E124" t="n">
-        <v>46.19400822808989</v>
+        <v>45.56567893959365</v>
       </c>
     </row>
     <row r="125">
@@ -2551,7 +2551,7 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>10728.00166298132</v>
+        <v>10728.00000253948</v>
       </c>
       <c r="C125" t="n">
         <v>0</v>
@@ -2560,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="E125" t="n">
-        <v>46.13425031616863</v>
+        <v>44.50701375816844</v>
       </c>
     </row>
     <row r="126">
@@ -2568,16 +2568,16 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>10804.99997002765</v>
+        <v>10804.99999985669</v>
       </c>
       <c r="C126" t="n">
-        <v>9.987725157313238e-06</v>
+        <v>4.74786252831145e-08</v>
       </c>
       <c r="D126" t="n">
-        <v>1.996467388299351e-05</v>
+        <v>9.573183063569892e-08</v>
       </c>
       <c r="E126" t="n">
-        <v>45.81454920213953</v>
+        <v>45.72090551443083</v>
       </c>
     </row>
     <row r="127">
@@ -2585,16 +2585,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>11149.99997958741</v>
+        <v>11150.00000150499</v>
       </c>
       <c r="C127" t="n">
-        <v>6.806097800972543e-06</v>
+        <v>0</v>
       </c>
       <c r="D127" t="n">
-        <v>1.359289587244437e-05</v>
+        <v>0</v>
       </c>
       <c r="E127" t="n">
-        <v>48.00167673036792</v>
+        <v>47.90831277941944</v>
       </c>
     </row>
     <row r="128">
@@ -2602,16 +2602,16 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>11858.99993265033</v>
+        <v>11858.99998064902</v>
       </c>
       <c r="C128" t="n">
-        <v>2.244067999611366e-05</v>
+        <v>6.430870472461782e-06</v>
       </c>
       <c r="D128" t="n">
-        <v>4.486414748585157e-05</v>
+        <v>1.290731291697866e-05</v>
       </c>
       <c r="E128" t="n">
-        <v>63.76199099714071</v>
+        <v>63.51454282451317</v>
       </c>
     </row>
     <row r="129">
@@ -2619,7 +2619,7 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>13069.38426915854</v>
+        <v>13069.38228809193</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
@@ -2628,7 +2628,7 @@
         <v>0</v>
       </c>
       <c r="E129" t="n">
-        <v>1911.867959378973</v>
+        <v>1536.475080420887</v>
       </c>
     </row>
     <row r="130">
@@ -2636,7 +2636,7 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>14238.74740819366</v>
+        <v>14238.74684722512</v>
       </c>
       <c r="C130" t="n">
         <v>0</v>
@@ -2645,7 +2645,7 @@
         <v>0</v>
       </c>
       <c r="E130" t="n">
-        <v>698.4954988860505</v>
+        <v>605.5020562441359</v>
       </c>
     </row>
     <row r="131">
@@ -2653,7 +2653,7 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>15002.00067212482</v>
+        <v>15002.06610439582</v>
       </c>
       <c r="C131" t="n">
         <v>0</v>
@@ -2662,7 +2662,7 @@
         <v>0</v>
       </c>
       <c r="E131" t="n">
-        <v>101.8068745076741</v>
+        <v>101.7540631319631</v>
       </c>
     </row>
     <row r="132">
@@ -2670,16 +2670,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>15236.01336226431</v>
+        <v>15235.98704203978</v>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>0.004317397422711393</v>
       </c>
       <c r="D132" t="n">
-        <v>0</v>
+        <v>0.008631932018936982</v>
       </c>
       <c r="E132" t="n">
-        <v>102.4095698126763</v>
+        <v>102.4076411315199</v>
       </c>
     </row>
     <row r="133">
@@ -2687,7 +2687,7 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>15213.15783196792</v>
+        <v>15213.1960390713</v>
       </c>
       <c r="C133" t="n">
         <v>0</v>
@@ -2696,7 +2696,7 @@
         <v>0</v>
       </c>
       <c r="E133" t="n">
-        <v>1051.444425144996</v>
+        <v>1041.545785155644</v>
       </c>
     </row>
     <row r="134">
@@ -2704,16 +2704,16 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>14949.99981189812</v>
+        <v>14950.00325551708</v>
       </c>
       <c r="C134" t="n">
-        <v>6.266926873111494e-05</v>
+        <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>0.0001253072788266432</v>
+        <v>0</v>
       </c>
       <c r="E134" t="n">
-        <v>74.07531898606928</v>
+        <v>74.07702860273277</v>
       </c>
     </row>
     <row r="135">
@@ -2721,16 +2721,16 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>14625.99996520061</v>
+        <v>14626.00078181541</v>
       </c>
       <c r="C135" t="n">
-        <v>1.159487430507266e-05</v>
+        <v>0</v>
       </c>
       <c r="D135" t="n">
-        <v>2.318132275364333e-05</v>
+        <v>0</v>
       </c>
       <c r="E135" t="n">
-        <v>73.00101265963784</v>
+        <v>73.00075949803299</v>
       </c>
     </row>
     <row r="136">
@@ -2738,16 +2738,16 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>14351.00004136457</v>
+        <v>14350.99999986192</v>
       </c>
       <c r="C136" t="n">
-        <v>0</v>
+        <v>1.243310792371996e-06</v>
       </c>
       <c r="D136" t="n">
-        <v>0</v>
+        <v>2.4161166437874e-06</v>
       </c>
       <c r="E136" t="n">
-        <v>71.28031657733534</v>
+        <v>71.28039393899759</v>
       </c>
     </row>
     <row r="137">
@@ -2755,16 +2755,16 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>14233.99998712387</v>
+        <v>14234.00003809872</v>
       </c>
       <c r="C137" t="n">
-        <v>4.26828202393416e-06</v>
+        <v>7.704904737482875e-07</v>
       </c>
       <c r="D137" t="n">
-        <v>8.599251121464881e-06</v>
+        <v>1.570598618655261e-06</v>
       </c>
       <c r="E137" t="n">
-        <v>70.90474956827694</v>
+        <v>70.90468564867697</v>
       </c>
     </row>
     <row r="138">
@@ -2772,16 +2772,16 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>14405.67581683608</v>
+        <v>14405.67556260382</v>
       </c>
       <c r="C138" t="n">
-        <v>76.32440771855482</v>
+        <v>76.32443631979183</v>
       </c>
       <c r="D138" t="n">
-        <v>0</v>
+        <v>1.075535815302979e-06</v>
       </c>
       <c r="E138" t="n">
-        <v>71.46577241378621</v>
+        <v>71.46660387273855</v>
       </c>
     </row>
     <row r="139">
@@ -2789,16 +2789,16 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>14717.92715267072</v>
+        <v>14717.94321861151</v>
       </c>
       <c r="C139" t="n">
-        <v>266.1202634166621</v>
+        <v>266.1189633706837</v>
       </c>
       <c r="D139" t="n">
         <v>0</v>
       </c>
       <c r="E139" t="n">
-        <v>81.9577834244152</v>
+        <v>82.21079321707442</v>
       </c>
     </row>
     <row r="140">
@@ -2806,16 +2806,16 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>14957.01547438161</v>
+        <v>14957.2646409569</v>
       </c>
       <c r="C140" t="n">
-        <v>673.9829433958735</v>
+        <v>673.9587074292135</v>
       </c>
       <c r="D140" t="n">
-        <v>0.001580641806994258</v>
+        <v>0</v>
       </c>
       <c r="E140" t="n">
-        <v>101.6887820127095</v>
+        <v>101.7417572624182</v>
       </c>
     </row>
     <row r="141">
@@ -2823,16 +2823,16 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>14601.67988565692</v>
+        <v>14601.54331051347</v>
       </c>
       <c r="C141" t="n">
-        <v>892.3654890685201</v>
+        <v>892.4159749747708</v>
       </c>
       <c r="D141" t="n">
-        <v>0</v>
+        <v>0.04315634529083288</v>
       </c>
       <c r="E141" t="n">
-        <v>101.8524343255614</v>
+        <v>101.7637882116788</v>
       </c>
     </row>
     <row r="142">
@@ -2840,16 +2840,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>14124.95494301655</v>
+        <v>14124.95618488319</v>
       </c>
       <c r="C142" t="n">
-        <v>844.0417184863095</v>
+        <v>844.0412044663997</v>
       </c>
       <c r="D142" t="n">
-        <v>0.003335162004886127</v>
+        <v>0.002627665285946746</v>
       </c>
       <c r="E142" t="n">
-        <v>101.7075001440621</v>
+        <v>71.63302287058521</v>
       </c>
     </row>
     <row r="143">
@@ -2857,16 +2857,16 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>13320.28558269288</v>
+        <v>13320.36470311321</v>
       </c>
       <c r="C143" t="n">
-        <v>877.713360694464</v>
+        <v>877.7069042778867</v>
       </c>
       <c r="D143" t="n">
-        <v>0.001055557138102675</v>
+        <v>0</v>
       </c>
       <c r="E143" t="n">
-        <v>71.99796658326729</v>
+        <v>70.45998814787049</v>
       </c>
     </row>
     <row r="144">
@@ -2874,16 +2874,16 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>12388.16748789197</v>
+        <v>12388.12901751106</v>
       </c>
       <c r="C144" t="n">
-        <v>790.8326374932324</v>
+        <v>790.8518505373487</v>
       </c>
       <c r="D144" t="n">
-        <v>0</v>
+        <v>0.01911284648795297</v>
       </c>
       <c r="E144" t="n">
-        <v>69.24268421184929</v>
+        <v>69.54146751615242</v>
       </c>
     </row>
     <row r="145">
@@ -2891,16 +2891,16 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>11366.41928101988</v>
+        <v>11366.41948602241</v>
       </c>
       <c r="C145" t="n">
-        <v>752.5807436098222</v>
+        <v>752.5807930021169</v>
       </c>
       <c r="D145" t="n">
-        <v>0</v>
+        <v>4.83633437103109e-05</v>
       </c>
       <c r="E145" t="n">
-        <v>51.10593959782171</v>
+        <v>51.10553973311563</v>
       </c>
     </row>
     <row r="146">
@@ -2908,16 +2908,16 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>10648.51171342556</v>
+        <v>10648.51186883741</v>
       </c>
       <c r="C146" t="n">
-        <v>548.4882345969087</v>
+        <v>548.4881980383575</v>
       </c>
       <c r="D146" t="n">
-        <v>5.192562129870663e-05</v>
+        <v>1.08009915412301e-05</v>
       </c>
       <c r="E146" t="n">
-        <v>47.63551843554749</v>
+        <v>47.63557788055454</v>
       </c>
     </row>
     <row r="147">
@@ -2925,16 +2925,16 @@
         <v>145</v>
       </c>
       <c r="B147" t="n">
-        <v>9515.036410840354</v>
+        <v>9515.036569137705</v>
       </c>
       <c r="C147" t="n">
-        <v>587.9635338595594</v>
+        <v>587.9634873103255</v>
       </c>
       <c r="D147" t="n">
-        <v>5.524485294538468e-05</v>
+        <v>5.909576975564101e-06</v>
       </c>
       <c r="E147" t="n">
-        <v>40.7987310239305</v>
+        <v>40.79885677073668</v>
       </c>
     </row>
     <row r="148">
@@ -2942,16 +2942,16 @@
         <v>146</v>
       </c>
       <c r="B148" t="n">
-        <v>9932.028945060825</v>
+        <v>9932.029776993781</v>
       </c>
       <c r="C148" t="n">
-        <v>678.9707821455531</v>
+        <v>678.9705003369763</v>
       </c>
       <c r="D148" t="n">
-        <v>0.0002725211101931301</v>
+        <v>0</v>
       </c>
       <c r="E148" t="n">
-        <v>44.39002732265709</v>
+        <v>44.41460562569353</v>
       </c>
     </row>
     <row r="149">
@@ -2959,16 +2959,16 @@
         <v>147</v>
       </c>
       <c r="B149" t="n">
-        <v>9511.9012664735</v>
+        <v>9511.882629616819</v>
       </c>
       <c r="C149" t="n">
-        <v>814.1165732332342</v>
+        <v>814.1176991941535</v>
       </c>
       <c r="D149" t="n">
         <v>0</v>
       </c>
       <c r="E149" t="n">
-        <v>41.53600190802339</v>
+        <v>41.53839944221978</v>
       </c>
     </row>
     <row r="150">
@@ -2976,16 +2976,16 @@
         <v>148</v>
       </c>
       <c r="B150" t="n">
-        <v>9796.94461663081</v>
+        <v>9796.902172396893</v>
       </c>
       <c r="C150" t="n">
-        <v>465.0954437884951</v>
+        <v>465.0979573407425</v>
       </c>
       <c r="D150" t="n">
-        <v>0</v>
+        <v>2.802196133642692e-05</v>
       </c>
       <c r="E150" t="n">
-        <v>44.36322475188928</v>
+        <v>44.31770936528166</v>
       </c>
     </row>
     <row r="151">
@@ -2993,16 +2993,16 @@
         <v>149</v>
       </c>
       <c r="B151" t="n">
-        <v>9384.062878588376</v>
+        <v>9384.063841681877</v>
       </c>
       <c r="C151" t="n">
-        <v>996.9394102266659</v>
+        <v>996.9393691524888</v>
       </c>
       <c r="D151" t="n">
         <v>0</v>
       </c>
       <c r="E151" t="n">
-        <v>40.83344179738649</v>
+        <v>40.83519504457685</v>
       </c>
     </row>
     <row r="152">
@@ -3010,16 +3010,16 @@
         <v>150</v>
       </c>
       <c r="B152" t="n">
-        <v>9479.458559631668</v>
+        <v>9479.462988165278</v>
       </c>
       <c r="C152" t="n">
-        <v>1197.541425546194</v>
+        <v>1197.541147182657</v>
       </c>
       <c r="D152" t="n">
-        <v>1.480733367496483e-05</v>
+        <v>0</v>
       </c>
       <c r="E152" t="n">
-        <v>40.69437854419188</v>
+        <v>40.69173677775941</v>
       </c>
     </row>
     <row r="153">
@@ -3027,16 +3027,16 @@
         <v>151</v>
       </c>
       <c r="B153" t="n">
-        <v>9914.587644553418</v>
+        <v>9914.585850818459</v>
       </c>
       <c r="C153" t="n">
-        <v>1259.412268628775</v>
+        <v>1259.413354367895</v>
       </c>
       <c r="D153" t="n">
-        <v>8.673110112312649e-05</v>
+        <v>0.001167146340015059</v>
       </c>
       <c r="E153" t="n">
-        <v>43.94377354191642</v>
+        <v>43.94158846652094</v>
       </c>
     </row>
     <row r="154">
@@ -3044,16 +3044,16 @@
         <v>152</v>
       </c>
       <c r="B154" t="n">
-        <v>11032.40788337693</v>
+        <v>11032.38671605457</v>
       </c>
       <c r="C154" t="n">
-        <v>1027.610602274238</v>
+        <v>1027.611358826409</v>
       </c>
       <c r="D154" t="n">
         <v>0</v>
       </c>
       <c r="E154" t="n">
-        <v>1215.670375258313</v>
+        <v>1329.930140015442</v>
       </c>
     </row>
     <row r="155">
@@ -3061,16 +3061,16 @@
         <v>153</v>
       </c>
       <c r="B155" t="n">
-        <v>12275.00845358136</v>
+        <v>12274.85889125111</v>
       </c>
       <c r="C155" t="n">
-        <v>679.9915183865787</v>
+        <v>680.0664943206689</v>
       </c>
       <c r="D155" t="n">
-        <v>2.800407042933334e-05</v>
+        <v>0.07453990639142635</v>
       </c>
       <c r="E155" t="n">
-        <v>69.47042561234288</v>
+        <v>69.41511318910771</v>
       </c>
     </row>
     <row r="156">
@@ -3078,16 +3078,16 @@
         <v>154</v>
       </c>
       <c r="B156" t="n">
-        <v>13139.21050400519</v>
+        <v>13139.52241244274</v>
       </c>
       <c r="C156" t="n">
-        <v>454.7898412652021</v>
+        <v>454.7681544773743</v>
       </c>
       <c r="D156" t="n">
         <v>0</v>
       </c>
       <c r="E156" t="n">
-        <v>69.85064624733162</v>
+        <v>69.95196133587376</v>
       </c>
     </row>
     <row r="157">
@@ -3095,16 +3095,16 @@
         <v>155</v>
       </c>
       <c r="B157" t="n">
-        <v>13761.63974333522</v>
+        <v>13761.63585981652</v>
       </c>
       <c r="C157" t="n">
-        <v>200.36025635894</v>
+        <v>200.3622034300362</v>
       </c>
       <c r="D157" t="n">
-        <v>3.055382424820211e-07</v>
+        <v>0.001934817886858453</v>
       </c>
       <c r="E157" t="n">
-        <v>70.49938947488268</v>
+        <v>70.50017187670184</v>
       </c>
     </row>
     <row r="158">
@@ -3112,7 +3112,7 @@
         <v>156</v>
       </c>
       <c r="B158" t="n">
-        <v>14101.8694495719</v>
+        <v>14101.86944746987</v>
       </c>
       <c r="C158" t="n">
         <v>0</v>
@@ -3121,7 +3121,7 @@
         <v>0</v>
       </c>
       <c r="E158" t="n">
-        <v>245.8380821691961</v>
+        <v>371.5905792060489</v>
       </c>
     </row>
     <row r="159">
@@ -3129,16 +3129,16 @@
         <v>157</v>
       </c>
       <c r="B159" t="n">
-        <v>14043.99998790571</v>
+        <v>14044.00209876313</v>
       </c>
       <c r="C159" t="n">
-        <v>3.962684602518184e-06</v>
+        <v>0</v>
       </c>
       <c r="D159" t="n">
-        <v>8.123525216553073e-06</v>
+        <v>0</v>
       </c>
       <c r="E159" t="n">
-        <v>70.84280916199397</v>
+        <v>70.84517825652482</v>
       </c>
     </row>
     <row r="160">
@@ -3146,16 +3146,16 @@
         <v>158</v>
       </c>
       <c r="B160" t="n">
-        <v>13897.00009400102</v>
+        <v>13896.99973233418</v>
       </c>
       <c r="C160" t="n">
-        <v>0</v>
+        <v>8.925286080950784e-05</v>
       </c>
       <c r="D160" t="n">
-        <v>0</v>
+        <v>0.0001782347671150687</v>
       </c>
       <c r="E160" t="n">
-        <v>70.6997122600857</v>
+        <v>70.69846626080007</v>
       </c>
     </row>
     <row r="161">
@@ -3163,7 +3163,7 @@
         <v>159</v>
       </c>
       <c r="B161" t="n">
-        <v>13818.00003781719</v>
+        <v>13818.00184385502</v>
       </c>
       <c r="C161" t="n">
         <v>0</v>
@@ -3172,7 +3172,7 @@
         <v>0</v>
       </c>
       <c r="E161" t="n">
-        <v>70.51142662080125</v>
+        <v>70.51152312983727</v>
       </c>
     </row>
     <row r="162">
@@ -3180,16 +3180,16 @@
         <v>160</v>
       </c>
       <c r="B162" t="n">
-        <v>14043.99959218409</v>
+        <v>14044.00061573572</v>
       </c>
       <c r="C162" t="n">
-        <v>0.0001356959431780937</v>
+        <v>0</v>
       </c>
       <c r="D162" t="n">
-        <v>0.0002718480475363989</v>
+        <v>0</v>
       </c>
       <c r="E162" t="n">
-        <v>70.715565000673</v>
+        <v>70.70662476139985</v>
       </c>
     </row>
     <row r="163">
@@ -3197,16 +3197,16 @@
         <v>161</v>
       </c>
       <c r="B163" t="n">
-        <v>14534.986900393</v>
+        <v>14534.99977870183</v>
       </c>
       <c r="C163" t="n">
-        <v>0.004194689256008122</v>
+        <v>7.510097969224533e-05</v>
       </c>
       <c r="D163" t="n">
-        <v>0.008896022107071858</v>
+        <v>0.0001460512282936555</v>
       </c>
       <c r="E163" t="n">
-        <v>82.16092888509918</v>
+        <v>93.54509471955326</v>
       </c>
     </row>
     <row r="164">
@@ -3214,16 +3214,16 @@
         <v>162</v>
       </c>
       <c r="B164" t="n">
-        <v>14997.05872924027</v>
+        <v>14996.99993656616</v>
       </c>
       <c r="C164" t="n">
-        <v>0</v>
+        <v>2.114155500771973e-05</v>
       </c>
       <c r="D164" t="n">
-        <v>0</v>
+        <v>4.22500205885047e-05</v>
       </c>
       <c r="E164" t="n">
-        <v>82.45529896259062</v>
+        <v>82.58591093444183</v>
       </c>
     </row>
     <row r="165">
@@ -3231,16 +3231,16 @@
         <v>163</v>
       </c>
       <c r="B165" t="n">
-        <v>15633.96729359237</v>
+        <v>15634.00013244592</v>
       </c>
       <c r="C165" t="n">
-        <v>0.01089735633045693</v>
+        <v>0</v>
       </c>
       <c r="D165" t="n">
-        <v>0.0217872653650176</v>
+        <v>0</v>
       </c>
       <c r="E165" t="n">
-        <v>103.4128607202917</v>
+        <v>103.4314337931942</v>
       </c>
     </row>
     <row r="166">
@@ -3248,7 +3248,7 @@
         <v>164</v>
       </c>
       <c r="B166" t="n">
-        <v>15558.12741722286</v>
+        <v>15558.81015684165</v>
       </c>
       <c r="C166" t="n">
         <v>0</v>
@@ -3257,7 +3257,7 @@
         <v>0</v>
       </c>
       <c r="E166" t="n">
-        <v>103.2094442521698</v>
+        <v>166.8173614211256</v>
       </c>
     </row>
     <row r="167">
@@ -3265,7 +3265,7 @@
         <v>165</v>
       </c>
       <c r="B167" t="n">
-        <v>14650.02487249774</v>
+        <v>14650.0000079258</v>
       </c>
       <c r="C167" t="n">
         <v>0</v>
@@ -3274,7 +3274,7 @@
         <v>0</v>
       </c>
       <c r="E167" t="n">
-        <v>73.05995492096358</v>
+        <v>73.05095388803589</v>
       </c>
     </row>
     <row r="168">
@@ -3282,7 +3282,7 @@
         <v>166</v>
       </c>
       <c r="B168" t="n">
-        <v>13470.01110675924</v>
+        <v>13470.00000840419</v>
       </c>
       <c r="C168" t="n">
         <v>0</v>
@@ -3291,7 +3291,7 @@
         <v>0</v>
       </c>
       <c r="E168" t="n">
-        <v>71.11614433212925</v>
+        <v>71.11386951034181</v>
       </c>
     </row>
     <row r="169">
@@ -3299,16 +3299,16 @@
         <v>167</v>
       </c>
       <c r="B169" t="n">
-        <v>12278.00012047601</v>
+        <v>12277.99999940275</v>
       </c>
       <c r="C169" t="n">
-        <v>0</v>
+        <v>1.977066207858514e-07</v>
       </c>
       <c r="D169" t="n">
-        <v>0</v>
+        <v>3.99144179342173e-07</v>
       </c>
       <c r="E169" t="n">
-        <v>101.2517664649671</v>
+        <v>101.2517082912324</v>
       </c>
     </row>
   </sheetData>

</xml_diff>